<commit_message>
created inject data from excel funtion
</commit_message>
<xml_diff>
--- a/api/fixtures/fixtures.xlsx
+++ b/api/fixtures/fixtures.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Roles" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Users" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Bans" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Role" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="User" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ban" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -176,7 +176,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -212,13 +212,6 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFA9B7C6"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,10 +272,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,66 +281,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFA9B7C6"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -458,7 +387,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -490,7 +419,6 @@
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="0"/>
       <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
@@ -706,7 +634,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J7" s="3" t="b">
+      <c r="J7" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -736,36 +665,39 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>